<commit_message>
FIX: typo in explanations.
</commit_message>
<xml_diff>
--- a/Data/Individual_data_expl.xlsx
+++ b/Data/Individual_data_expl.xlsx
@@ -238,7 +238,7 @@
     <t xml:space="preserve">Namų šeimininkas (-ė), kitas ekonomiškai neaktyvus asmuo</t>
   </si>
   <si>
-    <t xml:space="preserve">ME0908_1ž</t>
+    <t xml:space="preserve">ME0908_1z</t>
   </si>
   <si>
     <t xml:space="preserve">Pagrindinis darbas: profesija</t>
@@ -316,6 +316,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -336,6 +337,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -385,11 +387,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -518,8 +520,8 @@
   </sheetPr>
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
UPD: typo in explanations.
</commit_message>
<xml_diff>
--- a/Data/Individual_data_expl.xlsx
+++ b/Data/Individual_data_expl.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="95">
   <si>
     <t xml:space="preserve">Kintamojo pavadinimas</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lietuva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00</t>
   </si>
   <si>
     <t xml:space="preserve">Kita šalis</t>
@@ -308,8 +311,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -382,7 +386,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -393,6 +397,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -520,8 +528,8 @@
   </sheetPr>
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -577,11 +585,11 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="1" t="n">
-        <v>0</v>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,31 +599,31 @@
         <v>88</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="1" t="n">
-        <v>0</v>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,15 +633,15 @@
         <v>88</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
@@ -645,11 +653,11 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="1" t="n">
-        <v>0</v>
+      <c r="C11" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,7 +667,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,15 +677,15 @@
         <v>88</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>10</v>
@@ -689,11 +697,11 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="1" t="n">
-        <v>0</v>
+      <c r="C15" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,7 +711,7 @@
         <v>99</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,21 +721,21 @@
         <v>88</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,31 +745,31 @@
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -771,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,21 +799,21 @@
         <v>4</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -825,7 +833,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -835,51 +843,51 @@
         <v>8</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,7 +907,7 @@
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -909,7 +917,7 @@
         <v>4</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -919,7 +927,7 @@
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -929,21 +937,21 @@
         <v>6</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C38" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,7 +961,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,7 +971,7 @@
         <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,21 +981,21 @@
         <v>8</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,7 +1005,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,21 +1015,21 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,7 +1039,7 @@
         <v>2</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,7 +1049,7 @@
         <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1051,21 +1059,21 @@
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C49" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,7 +1083,7 @@
         <v>2</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,7 +1093,7 @@
         <v>3</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1095,7 +1103,7 @@
         <v>4</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,7 +1113,7 @@
         <v>5</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1115,7 +1123,7 @@
         <v>6</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,21 +1133,21 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,7 +1157,7 @@
         <v>2</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1159,7 +1167,7 @@
         <v>3</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1169,7 +1177,7 @@
         <v>4</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,7 +1187,7 @@
         <v>5</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1189,7 +1197,7 @@
         <v>6</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,7 +1207,7 @@
         <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,17 +1217,17 @@
         <v>8</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,7 +1237,7 @@
         <v>88</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1239,21 +1247,21 @@
         <v>99</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,7 +1271,7 @@
         <v>2</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,7 +1281,7 @@
         <v>3</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1283,7 +1291,7 @@
         <v>4</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,21 +1301,21 @@
         <v>8</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1317,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,7 +1335,7 @@
         <v>8</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>